<commit_message>
actualizacion del cronograma: diseño final completado
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDC/Documentos/SGDC_CP.xlsx
+++ b/Desarrollo/SGDC/Documentos/SGDC_CP.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Desktop\CodeMentorSolutions\Desarrollo\SGDC\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNMSM_Cursos\fisi_8vo_ciclo\Gest_conf_mantto\HernandezLivia\CodeMentorSolutions\Desarrollo\SGDC\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D25AD9-EE85-472A-8F5E-E0D78978E364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
@@ -527,7 +526,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -1703,26 +1702,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:K1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="41.21875" customWidth="1"/>
+    <col min="3" max="3" width="44.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" customWidth="1"/>
     <col min="6" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1">
@@ -1829,7 +1828,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:11" ht="47.25">
+    <row r="9" spans="1:11" ht="31.2">
       <c r="A9" s="12"/>
       <c r="B9" s="52" t="s">
         <v>9</v>
@@ -1854,7 +1853,7 @@
       </c>
       <c r="I9" s="54"/>
     </row>
-    <row r="10" spans="1:11" ht="38.25">
+    <row r="10" spans="1:11" ht="39.6">
       <c r="A10" s="12"/>
       <c r="B10" s="55" t="s">
         <v>16</v>
@@ -1880,7 +1879,7 @@
       <c r="I10" s="58"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="38.25">
+    <row r="11" spans="1:11" ht="39.6">
       <c r="A11" s="12"/>
       <c r="B11" s="55" t="s">
         <v>19</v>
@@ -1908,7 +1907,7 @@
       </c>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="38.25">
+    <row r="12" spans="1:11" ht="39.6">
       <c r="A12" s="12"/>
       <c r="B12" s="55" t="s">
         <v>21</v>
@@ -1937,7 +1936,7 @@
       <c r="J12" s="22"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="38.25">
+    <row r="13" spans="1:11" ht="39.6">
       <c r="A13" s="12"/>
       <c r="B13" s="55" t="s">
         <v>24</v>
@@ -2016,7 +2015,7 @@
       <c r="J15" s="22"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1">
+    <row r="16" spans="1:11" ht="13.2">
       <c r="A16" s="12"/>
       <c r="B16" s="55" t="s">
         <v>150</v>
@@ -2043,7 +2042,7 @@
       <c r="J16" s="22"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1">
+    <row r="17" spans="1:11" ht="13.2">
       <c r="A17" s="12"/>
       <c r="B17" s="55" t="s">
         <v>149</v>
@@ -2070,7 +2069,7 @@
       <c r="J17" s="22"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1">
+    <row r="18" spans="1:11" ht="26.4">
       <c r="A18" s="12"/>
       <c r="B18" s="55" t="s">
         <v>34</v>
@@ -2097,7 +2096,7 @@
       <c r="J18" s="22"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1">
+    <row r="19" spans="1:11" ht="26.4">
       <c r="A19" s="12"/>
       <c r="B19" s="55" t="s">
         <v>34</v>
@@ -2126,7 +2125,7 @@
       <c r="J19" s="22"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1">
+    <row r="20" spans="1:11" ht="26.4">
       <c r="A20" s="12"/>
       <c r="B20" s="55" t="s">
         <v>34</v>
@@ -2153,7 +2152,7 @@
       <c r="J20" s="22"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1">
+    <row r="21" spans="1:11" ht="26.4">
       <c r="A21" s="12"/>
       <c r="B21" s="55" t="s">
         <v>34</v>
@@ -2180,7 +2179,7 @@
       <c r="J21" s="22"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1">
+    <row r="22" spans="1:11" ht="26.4">
       <c r="A22" s="12"/>
       <c r="B22" s="55" t="s">
         <v>34</v>
@@ -2207,7 +2206,7 @@
       <c r="J22" s="22"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1">
+    <row r="23" spans="1:11" ht="26.4">
       <c r="A23" s="12"/>
       <c r="B23" s="55" t="s">
         <v>34</v>
@@ -2234,7 +2233,7 @@
       <c r="J23" s="22"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1">
+    <row r="24" spans="1:11" ht="26.4">
       <c r="A24" s="12"/>
       <c r="B24" s="55" t="s">
         <v>34</v>
@@ -2261,7 +2260,7 @@
       <c r="J24" s="22"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1">
+    <row r="25" spans="1:11" ht="26.4">
       <c r="A25" s="12"/>
       <c r="B25" s="55" t="s">
         <v>34</v>
@@ -2288,7 +2287,7 @@
       <c r="J25" s="22"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1">
+    <row r="26" spans="1:11" ht="26.4">
       <c r="A26" s="12"/>
       <c r="B26" s="55" t="s">
         <v>34</v>
@@ -2315,7 +2314,7 @@
       <c r="J26" s="22"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1">
+    <row r="27" spans="1:11" ht="26.4">
       <c r="A27" s="12"/>
       <c r="B27" s="55" t="s">
         <v>60</v>
@@ -2425,7 +2424,7 @@
       <c r="J30" s="22"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="12.75">
+    <row r="31" spans="1:11" ht="13.2">
       <c r="A31" s="12"/>
       <c r="B31" s="55" t="s">
         <v>73</v>
@@ -2452,7 +2451,7 @@
       <c r="J31" s="22"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="12.75">
+    <row r="32" spans="1:11" ht="13.2">
       <c r="A32" s="12"/>
       <c r="B32" s="55" t="s">
         <v>75</v>
@@ -2479,7 +2478,7 @@
       <c r="J32" s="22"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="38.25">
+    <row r="33" spans="1:11" ht="39.6">
       <c r="A33" s="12"/>
       <c r="B33" s="55" t="s">
         <v>136</v>
@@ -2506,7 +2505,7 @@
       <c r="J33" s="22"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="38.25">
+    <row r="34" spans="1:11" ht="39.6">
       <c r="A34" s="12"/>
       <c r="B34" s="55" t="s">
         <v>137</v>
@@ -2533,7 +2532,7 @@
       <c r="J34" s="22"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="25.5">
+    <row r="35" spans="1:11" ht="26.4">
       <c r="A35" s="12" t="s">
         <v>76</v>
       </c>
@@ -2600,7 +2599,7 @@
         <v>45070</v>
       </c>
       <c r="H37" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="90"/>
       <c r="J37" s="22"/>
@@ -2633,7 +2632,7 @@
       <c r="J38" s="22"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="25.5">
+    <row r="39" spans="1:11" ht="26.4">
       <c r="A39" s="12"/>
       <c r="B39" s="55" t="s">
         <v>79</v>
@@ -2687,7 +2686,7 @@
       <c r="J40" s="22"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="14.25">
+    <row r="41" spans="1:11" ht="13.8">
       <c r="A41" s="12"/>
       <c r="B41" s="72" t="s">
         <v>124</v>
@@ -2714,7 +2713,7 @@
       <c r="J41" s="22"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="14.25">
+    <row r="42" spans="1:11" ht="13.8">
       <c r="A42" s="12"/>
       <c r="B42" s="55" t="s">
         <v>81</v>
@@ -2741,7 +2740,7 @@
       <c r="J42" s="22"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" ht="38.25">
+    <row r="43" spans="1:11" ht="39.6">
       <c r="A43" s="12"/>
       <c r="B43" s="55" t="s">
         <v>138</v>
@@ -2770,7 +2769,7 @@
       <c r="J43" s="22"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="38.25">
+    <row r="44" spans="1:11" ht="39.6">
       <c r="A44" s="12"/>
       <c r="B44" s="55" t="s">
         <v>139</v>
@@ -2797,7 +2796,7 @@
       <c r="J44" s="22"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" ht="25.5">
+    <row r="45" spans="1:11" ht="26.4">
       <c r="A45" s="12" t="s">
         <v>83</v>
       </c>
@@ -2843,7 +2842,7 @@
       <c r="J46" s="22"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="25.5">
+    <row r="47" spans="1:11" ht="26.4">
       <c r="A47" s="12"/>
       <c r="B47" s="55" t="s">
         <v>88</v>
@@ -2870,7 +2869,7 @@
       <c r="J47" s="22"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="14.25">
+    <row r="48" spans="1:11" ht="13.8">
       <c r="A48" s="12"/>
       <c r="B48" s="55" t="s">
         <v>89</v>
@@ -2897,7 +2896,7 @@
       <c r="J48" s="22"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="14.25">
+    <row r="49" spans="1:11" ht="13.8">
       <c r="A49" s="12"/>
       <c r="B49" s="75" t="s">
         <v>85</v>
@@ -2924,7 +2923,7 @@
       <c r="J49" s="22"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" ht="38.25">
+    <row r="50" spans="1:11" ht="39.6">
       <c r="A50" s="12"/>
       <c r="B50" s="55" t="s">
         <v>140</v>
@@ -2951,7 +2950,7 @@
       <c r="J50" s="22"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="38.25">
+    <row r="51" spans="1:11" ht="39.6">
       <c r="A51" s="12"/>
       <c r="B51" s="55" t="s">
         <v>141</v>
@@ -2980,7 +2979,7 @@
       <c r="J51" s="22"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" ht="38.25">
+    <row r="52" spans="1:11" ht="39.6">
       <c r="A52" s="12"/>
       <c r="B52" s="76" t="s">
         <v>91</v>
@@ -3007,7 +3006,7 @@
       <c r="J52" s="22"/>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:11" ht="25.5">
+    <row r="53" spans="1:11" ht="26.4">
       <c r="A53" s="12" t="s">
         <v>94</v>
       </c>
@@ -8217,7 +8216,7 @@
     <mergeCell ref="I33:I35"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId2"/>
@@ -8225,7 +8224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -8235,12 +8234,12 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1"/>
@@ -9362,7 +9361,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -9370,9 +9369,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="12.7109375" customWidth="1"/>
+    <col min="1" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
subiendo el acta de cierre del proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDC/Documentos/SGDC_CP.xlsx
+++ b/Desarrollo/SGDC/Documentos/SGDC_CP.xlsx
@@ -1655,8 +1655,8 @@
   </sheetPr>
   <dimension ref="A1:K1008"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -2947,7 +2947,7 @@
         <v>45107</v>
       </c>
       <c r="H52" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" s="87"/>
       <c r="J52" s="22"/>

</xml_diff>

<commit_message>
subiendo las actas finales
</commit_message>
<xml_diff>
--- a/Desarrollo/SGDC/Documentos/SGDC_CP.xlsx
+++ b/Desarrollo/SGDC/Documentos/SGDC_CP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNMSM_Cursos\fisi_8vo_ciclo\Gest_conf_mantto\HernandezLivia\CodeMentorSolutions\Desarrollo\SGDC\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fisi_UNMSM\fisi_8vo_ciclo\Gest_conf_mantto\HernandezLivia\CodeMentorSolutions\Desarrollo\SGDC\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1656,7 +1656,7 @@
   <dimension ref="A1:K1008"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="H47" sqref="H47:H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -2783,7 +2783,7 @@
         <v>45081</v>
       </c>
       <c r="H46" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" s="55"/>
       <c r="J46" s="22"/>
@@ -2810,7 +2810,7 @@
         <v>45103</v>
       </c>
       <c r="H47" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47" s="55"/>
       <c r="J47" s="22"/>
@@ -2837,7 +2837,7 @@
         <v>45104</v>
       </c>
       <c r="H48" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48" s="55"/>
       <c r="J48" s="22"/>
@@ -2864,7 +2864,7 @@
         <v>45104</v>
       </c>
       <c r="H49" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" s="55"/>
       <c r="J49" s="22"/>
@@ -2891,7 +2891,7 @@
         <v>45105</v>
       </c>
       <c r="H50" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" s="55"/>
       <c r="J50" s="22"/>
@@ -2918,7 +2918,7 @@
         <v>45105</v>
       </c>
       <c r="H51" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="86" t="s">
         <v>90</v>
@@ -2947,7 +2947,7 @@
         <v>45106</v>
       </c>
       <c r="H52" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" s="87"/>
       <c r="J52" s="22"/>

</xml_diff>